<commit_message>
Handle renamed 't3*' questions for 2017
</commit_message>
<xml_diff>
--- a/data/OBS2017_QuestionsNumbers+Text.xlsx
+++ b/data/OBS2017_QuestionsNumbers+Text.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Y_Open Knowledge Data\for open knowledge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brew/Documents/Work/OpenKnowledge/ibp/ibp-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="880" windowWidth="31820" windowHeight="19900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
     <sheet name="2017" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1948,27 +1956,6 @@
   </si>
   <si>
     <t>Does not release to the public, or is released more than 18 months after the end of the budget year</t>
-  </si>
-  <si>
-    <t>t3pbs/PBS-2</t>
-  </si>
-  <si>
-    <t>t3ebp/EBP-2</t>
-  </si>
-  <si>
-    <t>t3eb/EB-2</t>
-  </si>
-  <si>
-    <t>t3iyr/IYR-2</t>
-  </si>
-  <si>
-    <t>t3myr/MYR-2</t>
-  </si>
-  <si>
-    <t>t3yer/YER-2</t>
-  </si>
-  <si>
-    <t>t3ar/AR-2</t>
   </si>
   <si>
     <t xml:space="preserve">Is there an Independent Fiscal Institution (IFI) that conducts budget analyses for the budget formulation and/or approval process? </t>
@@ -2445,6 +2432,27 @@
   </si>
   <si>
     <t>Yes, SAI maintains formal mechanisms through which the public can contribute to audit investigations.</t>
+  </si>
+  <si>
+    <t>PBS-2</t>
+  </si>
+  <si>
+    <t>EBP-2</t>
+  </si>
+  <si>
+    <t>EB-2</t>
+  </si>
+  <si>
+    <t>IYR-2</t>
+  </si>
+  <si>
+    <t>MYR-2</t>
+  </si>
+  <si>
+    <t>YER-2</t>
+  </si>
+  <si>
+    <t>AR-2</t>
   </si>
 </sst>
 </file>
@@ -2483,16 +2491,16 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2586,9 +2594,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -2621,9 +2629,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2805,23 +2813,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK141"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1"/>
-    <col min="2" max="2" width="25.5703125" style="1"/>
-    <col min="3" max="3" width="20.85546875" style="1"/>
-    <col min="4" max="4" width="24.85546875" style="1"/>
-    <col min="5" max="5" width="23.42578125" style="1"/>
-    <col min="6" max="6" width="19.42578125" style="1"/>
-    <col min="7" max="7" width="19.140625" style="1"/>
-    <col min="8" max="1025" width="8.7109375" style="1"/>
+    <col min="1" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2844,7 +2845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="325" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2867,7 +2868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="221" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2886,7 +2887,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2905,7 +2906,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="221" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2924,7 +2925,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2943,7 +2944,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="221" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2989,7 +2990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="299" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3012,7 +3013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="403" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3077,7 +3078,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3192,7 +3193,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="351" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3215,7 +3216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="403" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3261,7 +3262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="273" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3284,7 +3285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="364" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3303,7 +3304,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3326,7 +3327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3349,7 +3350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="273" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3372,7 +3373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="299" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3391,7 +3392,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="273" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3414,7 +3415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3433,7 +3434,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3452,7 +3453,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="299" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3475,7 +3476,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="273" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3498,7 +3499,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="267.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="273" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3567,7 +3568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3586,7 +3587,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3632,7 +3633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3678,7 +3679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="390" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="351" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3724,7 +3725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="234" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3747,7 +3748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3770,7 +3771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="229.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3793,7 +3794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3816,7 +3817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3839,7 +3840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3862,7 +3863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="364" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3885,7 +3886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3908,7 +3909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3931,7 +3932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="273" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3954,7 +3955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="221" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3977,7 +3978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4000,7 +4001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4023,7 +4024,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4046,7 +4047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4069,7 +4070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4092,7 +4093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4115,7 +4116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="221" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4134,7 +4135,7 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4157,7 +4158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4180,7 +4181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="143" x14ac:dyDescent="0.15">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4199,7 +4200,7 @@
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4222,7 +4223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4245,7 +4246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4268,7 +4269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="325" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="351" x14ac:dyDescent="0.15">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -4314,7 +4315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="273" x14ac:dyDescent="0.15">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -4337,7 +4338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -4360,7 +4361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="208" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -4383,7 +4384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -4402,7 +4403,7 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="143" x14ac:dyDescent="0.15">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -4421,7 +4422,7 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -4463,7 +4464,7 @@
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -4486,7 +4487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -4509,7 +4510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -4555,7 +4556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -4601,7 +4602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -4624,7 +4625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="169" x14ac:dyDescent="0.15">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -4643,7 +4644,7 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -4689,7 +4690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="299" x14ac:dyDescent="0.15">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -4735,7 +4736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -4781,7 +4782,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="143" x14ac:dyDescent="0.15">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -4800,7 +4801,7 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -4823,7 +4824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="351" x14ac:dyDescent="0.15">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -4846,7 +4847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -4869,7 +4870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="299" x14ac:dyDescent="0.15">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -4892,7 +4893,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="299" x14ac:dyDescent="0.15">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -4915,7 +4916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="403" x14ac:dyDescent="0.15">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -4938,7 +4939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -4961,7 +4962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="169" x14ac:dyDescent="0.15">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -4980,7 +4981,7 @@
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -5003,7 +5004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -5026,7 +5027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -5049,7 +5050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="182" x14ac:dyDescent="0.15">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5068,7 +5069,7 @@
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -5091,7 +5092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -5114,7 +5115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -5137,7 +5138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="390" x14ac:dyDescent="0.15">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -5183,7 +5184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -5206,7 +5207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -5229,7 +5230,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="182" x14ac:dyDescent="0.15">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -5252,7 +5253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="403" x14ac:dyDescent="0.15">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -5275,7 +5276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="403" x14ac:dyDescent="0.15">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -5298,7 +5299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="390" x14ac:dyDescent="0.15">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -5321,7 +5322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -5340,7 +5341,7 @@
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
     </row>
-    <row r="114" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="390" x14ac:dyDescent="0.15">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -5363,7 +5364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -5386,7 +5387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="169" x14ac:dyDescent="0.15">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -5409,7 +5410,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -5432,7 +5433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -5451,7 +5452,7 @@
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
     </row>
-    <row r="119" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -5474,7 +5475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -5497,7 +5498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -5520,7 +5521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -5543,7 +5544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="403" x14ac:dyDescent="0.15">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -5566,7 +5567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -5589,7 +5590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -5635,7 +5636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="325" x14ac:dyDescent="0.15">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -5658,7 +5659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="338" x14ac:dyDescent="0.15">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -5681,7 +5682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="325" x14ac:dyDescent="0.15">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -5704,7 +5705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" ht="182" x14ac:dyDescent="0.15">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -5727,7 +5728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" ht="351" x14ac:dyDescent="0.15">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -5750,7 +5751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" ht="312" x14ac:dyDescent="0.15">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -5773,7 +5774,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" ht="409" x14ac:dyDescent="0.15">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -5792,7 +5793,7 @@
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
     </row>
-    <row r="134" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" ht="286" x14ac:dyDescent="0.15">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -5815,7 +5816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" ht="299" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
         <v>596</v>
       </c>
@@ -5835,7 +5836,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
         <v>602</v>
       </c>
@@ -5855,7 +5856,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" ht="182" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
         <v>608</v>
       </c>
@@ -5875,7 +5876,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
         <v>614</v>
       </c>
@@ -5895,7 +5896,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" ht="234" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
         <v>620</v>
       </c>
@@ -5915,7 +5916,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" ht="182" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
         <v>626</v>
       </c>
@@ -5935,7 +5936,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
         <v>632</v>
       </c>
@@ -5965,18 +5966,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I124" sqref="I124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="7" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8" max="1025" width="9.140625" style="1"/>
+    <col min="1" max="7" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5999,7 +6000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6022,7 +6023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6041,7 +6042,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -6060,7 +6061,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -6079,7 +6080,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -6098,7 +6099,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -6121,7 +6122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -6144,7 +6145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -6190,7 +6191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -6213,7 +6214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -6232,7 +6233,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -6255,7 +6256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -6278,7 +6279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="169" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -6301,7 +6302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="182" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -6324,7 +6325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="182" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -6347,7 +6348,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -6370,7 +6371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -6393,7 +6394,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -6416,7 +6417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -6439,7 +6440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -6458,7 +6459,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -6481,7 +6482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -6504,7 +6505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -6527,7 +6528,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -6546,7 +6547,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -6569,7 +6570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -6588,7 +6589,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -6607,7 +6608,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -6630,7 +6631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -6653,7 +6654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="267.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -6676,7 +6677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -6699,7 +6700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="169" x14ac:dyDescent="0.15">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -6722,7 +6723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -6741,7 +6742,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -6764,7 +6765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -6787,7 +6788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -6810,7 +6811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -6833,7 +6834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -6856,7 +6857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -6879,7 +6880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -6902,7 +6903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="260" x14ac:dyDescent="0.15">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -6925,7 +6926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="229.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="208" x14ac:dyDescent="0.15">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -6948,7 +6949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -6971,7 +6972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -6994,7 +6995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -7017,7 +7018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -7040,7 +7041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -7063,7 +7064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -7086,7 +7087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -7109,7 +7110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -7132,7 +7133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -7155,7 +7156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="169" x14ac:dyDescent="0.15">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -7178,7 +7179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -7201,7 +7202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="169" x14ac:dyDescent="0.15">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -7224,7 +7225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -7247,7 +7248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -7270,7 +7271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -7289,7 +7290,7 @@
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -7312,7 +7313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -7335,7 +7336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -7354,7 +7355,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -7377,7 +7378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -7400,7 +7401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="143" x14ac:dyDescent="0.15">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -7423,7 +7424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -7446,7 +7447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -7469,7 +7470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -7492,7 +7493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -7515,7 +7516,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -7538,7 +7539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -7557,7 +7558,7 @@
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -7576,7 +7577,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
     </row>
-    <row r="73" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -7599,7 +7600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -7618,7 +7619,7 @@
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -7641,7 +7642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -7687,7 +7688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -7710,7 +7711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -7733,7 +7734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -7756,7 +7757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -7779,7 +7780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -7798,7 +7799,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -7821,7 +7822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -7844,7 +7845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -7867,7 +7868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -7890,7 +7891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -7913,7 +7914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -7936,7 +7937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -7955,7 +7956,7 @@
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
     </row>
-    <row r="90" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -7978,7 +7979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="104" x14ac:dyDescent="0.15">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -8001,7 +8002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -8024,7 +8025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -8047,7 +8048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -8070,7 +8071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -8093,7 +8094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -8116,7 +8117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -8135,7 +8136,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
     </row>
-    <row r="98" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -8158,7 +8159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -8181,7 +8182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -8204,7 +8205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -8223,7 +8224,7 @@
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
     </row>
-    <row r="102" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -8246,7 +8247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -8269,113 +8270,113 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A104" s="5">
         <v>103</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="G104" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A105" s="5">
         <v>104</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="G105" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A106" s="5">
         <v>105</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="G106" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A107" s="5">
         <v>106</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="G107" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A108" s="5">
         <v>107</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>460</v>
@@ -8384,7 +8385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -8401,13 +8402,13 @@
         <v>469</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -8430,7 +8431,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -8453,202 +8454,202 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A112" s="5">
         <v>111</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="G112" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A113" s="5">
         <v>112</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="G113" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A114" s="5">
         <v>113</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="G114" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A115" s="5">
         <v>114</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="G115" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A116" s="5">
         <v>115</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
       <c r="G116" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A117" s="5">
         <v>116</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A118" s="5">
         <v>117</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="G118" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A119" s="5">
         <v>118</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="G119" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A120" s="5">
         <v>119</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>12</v>
@@ -8656,7 +8657,7 @@
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -8675,7 +8676,7 @@
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="1:7" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="156" x14ac:dyDescent="0.15">
       <c r="A122" s="5">
         <v>121</v>
       </c>
@@ -8683,13 +8684,13 @@
         <v>522</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>524</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>526</v>
@@ -8698,7 +8699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -8721,87 +8722,87 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A124" s="5">
         <v>123</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>715</v>
+        <v>708</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>716</v>
+        <v>709</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="G124" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A125" s="5">
         <v>124</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="G125" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A126" s="5">
         <v>125</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>722</v>
+        <v>715</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G126" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A127" s="5">
         <v>126</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>726</v>
+        <v>719</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>12</v>
@@ -8809,64 +8810,64 @@
       <c r="F127" s="5"/>
       <c r="G127" s="3"/>
     </row>
-    <row r="128" spans="1:7" ht="229.5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="195" x14ac:dyDescent="0.15">
       <c r="A128" s="5">
         <v>127</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>730</v>
+        <v>723</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G128" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="130" x14ac:dyDescent="0.15">
       <c r="A129" s="5">
         <v>128</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>733</v>
+        <v>726</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>734</v>
+        <v>727</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G129" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" ht="117" x14ac:dyDescent="0.15">
       <c r="A130" s="5">
         <v>129</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>737</v>
+        <v>730</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>12</v>
@@ -8874,110 +8875,110 @@
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="1:7" ht="267.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" ht="247" x14ac:dyDescent="0.15">
       <c r="A131" s="5">
         <v>130</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>739</v>
+        <v>732</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>730</v>
+        <v>723</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>740</v>
+        <v>733</v>
       </c>
       <c r="G131" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="216.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" ht="221" x14ac:dyDescent="0.15">
       <c r="A132" s="5">
         <v>131</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>742</v>
+        <v>735</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>744</v>
+        <v>737</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G132" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" ht="91" x14ac:dyDescent="0.15">
       <c r="A133" s="5">
         <v>132</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>746</v>
+        <v>739</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>747</v>
+        <v>740</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>748</v>
+        <v>741</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G133" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="1" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" s="1" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A134" s="5">
         <v>133</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>750</v>
+        <v>743</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>751</v>
+        <v>744</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>748</v>
+        <v>741</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G134" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:7" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A135" s="5">
         <v>134</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>753</v>
+        <v>746</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>12</v>
@@ -8985,133 +8986,133 @@
       <c r="F135" s="5"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="1:7" s="1" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" s="1" customFormat="1" ht="130" x14ac:dyDescent="0.15">
       <c r="A136" s="5">
         <v>135</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>754</v>
+        <v>747</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>755</v>
+        <v>748</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>756</v>
+        <v>749</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G136" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:7" s="1" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" s="1" customFormat="1" ht="143" x14ac:dyDescent="0.15">
       <c r="A137" s="5">
         <v>136</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G137" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:7" s="1" customFormat="1" ht="267.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" s="1" customFormat="1" ht="247" x14ac:dyDescent="0.15">
       <c r="A138" s="5">
         <v>137</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G138" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:7" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" s="1" customFormat="1" ht="91" x14ac:dyDescent="0.15">
       <c r="A139" s="5">
         <v>138</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G139" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:7" s="1" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" s="1" customFormat="1" ht="156" x14ac:dyDescent="0.15">
       <c r="A140" s="5">
         <v>139</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>771</v>
+        <v>764</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>772</v>
+        <v>765</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>773</v>
+        <v>766</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G140" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:7" s="1" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" s="1" customFormat="1" ht="117" x14ac:dyDescent="0.15">
       <c r="A141" s="5">
         <v>140</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>775</v>
+        <v>768</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>12</v>
@@ -9119,41 +9120,41 @@
       <c r="F141" s="5"/>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="1:7" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A142" s="5">
         <v>141</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>776</v>
+        <v>769</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>777</v>
+        <v>770</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>778</v>
+        <v>771</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>779</v>
+        <v>772</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="G142" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:7" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A143" s="5">
         <v>142</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>780</v>
+        <v>773</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>781</v>
+        <v>774</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>12</v>
@@ -9161,9 +9162,9 @@
       <c r="F143" s="5"/>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="1:7" s="1" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A144" s="6" t="s">
-        <v>637</v>
+        <v>775</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>597</v>
@@ -9182,9 +9183,9 @@
       </c>
       <c r="G144" s="7"/>
     </row>
-    <row r="145" spans="1:7" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A145" s="6" t="s">
-        <v>638</v>
+        <v>776</v>
       </c>
       <c r="B145" s="7" t="s">
         <v>603</v>
@@ -9203,9 +9204,9 @@
       </c>
       <c r="G145" s="7"/>
     </row>
-    <row r="146" spans="1:7" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A146" s="6" t="s">
-        <v>639</v>
+        <v>777</v>
       </c>
       <c r="B146" s="7" t="s">
         <v>609</v>
@@ -9224,9 +9225,9 @@
       </c>
       <c r="G146" s="7"/>
     </row>
-    <row r="147" spans="1:7" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" s="1" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A147" s="6" t="s">
-        <v>640</v>
+        <v>778</v>
       </c>
       <c r="B147" s="7" t="s">
         <v>615</v>
@@ -9245,9 +9246,9 @@
       </c>
       <c r="G147" s="7"/>
     </row>
-    <row r="148" spans="1:7" s="1" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A148" s="6" t="s">
-        <v>641</v>
+        <v>779</v>
       </c>
       <c r="B148" s="7" t="s">
         <v>621</v>
@@ -9266,9 +9267,9 @@
       </c>
       <c r="G148" s="7"/>
     </row>
-    <row r="149" spans="1:7" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.15">
       <c r="A149" s="6" t="s">
-        <v>642</v>
+        <v>780</v>
       </c>
       <c r="B149" s="7" t="s">
         <v>627</v>
@@ -9287,9 +9288,9 @@
       </c>
       <c r="G149" s="7"/>
     </row>
-    <row r="150" spans="1:7" s="1" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.15">
       <c r="A150" s="6" t="s">
-        <v>643</v>
+        <v>781</v>
       </c>
       <c r="B150" s="7" t="s">
         <v>633</v>

</xml_diff>